<commit_message>
Edit and first run
</commit_message>
<xml_diff>
--- a/data/mapasEtiquetas.xlsx
+++ b/data/mapasEtiquetas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20820"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D88A20E-9F04-40F3-8B59-9BF6AED7C1BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB32C9EC-A8A3-4929-98A8-257F8C3667D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>./data/datosDepSuicidio.xlsx</t>
   </si>
   <si>
-    <t>./plots/MapaSuicidio.png</t>
+    <t>./plots/MapaSuicidio2009-2018.png</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +386,7 @@
     <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>